<commit_message>
Uploading project plan and updating test cases
Uploading project plan and updating test cases
</commit_message>
<xml_diff>
--- a/HarvestSwap_final/HarvestSwap TestCases.xlsx
+++ b/HarvestSwap_final/HarvestSwap TestCases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="150">
   <si>
     <t>Project Name:</t>
   </si>
@@ -328,7 +328,10 @@
     <t>Verify that the harvester can reach the My Profile page</t>
   </si>
   <si>
-    <t>Date and Time of Test: 12/7/2020; 4:30 pm</t>
+    <t>d5ac92e27363d40a7bbd990af14b75764766e427</t>
+  </si>
+  <si>
+    <t>Date and Time of Test: 12/7/2020; 12:45 AM</t>
   </si>
   <si>
     <t xml:space="preserve">1. Navigate to Harvest Swap web application                                                                                 2. User should be registered to the system.
@@ -466,7 +469,10 @@
     <t xml:space="preserve">Verify that the user has access to the add listing page </t>
   </si>
   <si>
-    <t>ea5d8c6</t>
+    <t>ea5d8c62b77e2a61bf1fbc8edcf1dc2291ec3320</t>
+  </si>
+  <si>
+    <t>Date and Time of Test: 12/06/2020; 1:15 PM</t>
   </si>
   <si>
     <t>1.User has the ability to create an account
@@ -493,6 +499,9 @@
   </si>
   <si>
     <t>Verfiy that the user can enter their information and submit it</t>
+  </si>
+  <si>
+    <t>ea5d8c62b77e2a61bf1fbc8edcf1dc2291ec3321</t>
   </si>
   <si>
     <t>1.User should have been able to make an account
@@ -519,6 +528,9 @@
     <t>Verify that the user is able to see their information on the swap center page and that the information stored in the database</t>
   </si>
   <si>
+    <t>ea5d8c62b77e2a61bf1fbc8edcf1dc2291ec3322</t>
+  </si>
+  <si>
     <t>1.User should have the access to the URL.       2. User should already have an account
 3. User should have already entered harvest info
 4. User should be logged in to the system.</t>
@@ -536,6 +548,9 @@
   </si>
   <si>
     <t>T020</t>
+  </si>
+  <si>
+    <t>ea5d8c62b77e2a61bf1fbc8edcf1dc2291ec3323</t>
   </si>
   <si>
     <t>1.User should have the access to the URL: 
@@ -1744,21 +1759,23 @@
       <c r="F16" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="G16" s="22"/>
+      <c r="G16" s="22" t="s">
+        <v>91</v>
+      </c>
       <c r="H16" s="23" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I16" s="24" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J16" s="25" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="K16" s="24" t="s">
         <v>43</v>
       </c>
       <c r="L16" s="26" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="M16" s="20" t="s">
         <v>37</v>
@@ -1787,7 +1804,7 @@
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
       <c r="C17" s="20" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D17" s="21" t="s">
         <v>28</v>
@@ -1796,23 +1813,25 @@
         <v>89</v>
       </c>
       <c r="F17" s="22" t="s">
-        <v>96</v>
-      </c>
-      <c r="G17" s="22"/>
+        <v>97</v>
+      </c>
+      <c r="G17" s="22" t="s">
+        <v>91</v>
+      </c>
       <c r="H17" s="23" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I17" s="24" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="J17" s="25" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="K17" s="24" t="s">
         <v>43</v>
       </c>
       <c r="L17" s="26" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="M17" s="20" t="s">
         <v>37</v>
@@ -1841,32 +1860,34 @@
       <c r="A18" s="28"/>
       <c r="B18" s="28"/>
       <c r="C18" s="29" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D18" s="30" t="s">
         <v>28</v>
       </c>
       <c r="E18" s="31" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F18" s="31" t="s">
-        <v>102</v>
-      </c>
-      <c r="G18" s="31"/>
+        <v>103</v>
+      </c>
+      <c r="G18" s="31" t="s">
+        <v>91</v>
+      </c>
       <c r="H18" s="32" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I18" s="33" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="J18" s="34" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="K18" s="33" t="s">
         <v>43</v>
       </c>
       <c r="L18" s="35" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="M18" s="29" t="s">
         <v>37</v>
@@ -1893,13 +1914,13 @@
     </row>
     <row r="19">
       <c r="A19" s="37" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B19" s="40" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D19" s="21" t="s">
         <v>28</v>
@@ -1908,25 +1929,25 @@
         <v>60</v>
       </c>
       <c r="F19" s="22" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G19" s="22" t="s">
         <v>31</v>
       </c>
       <c r="H19" s="23" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="I19" s="24" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="J19" s="25" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="K19" s="24" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="L19" s="26" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="M19" s="20" t="s">
         <v>37</v>
@@ -1955,7 +1976,7 @@
       <c r="A20" s="8"/>
       <c r="B20" s="8"/>
       <c r="C20" s="20" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D20" s="21" t="s">
         <v>28</v>
@@ -1964,25 +1985,25 @@
         <v>60</v>
       </c>
       <c r="F20" s="22" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G20" s="22" t="s">
         <v>31</v>
       </c>
       <c r="H20" s="23" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="I20" s="24" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="J20" s="25" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="K20" s="24" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="L20" s="26" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="M20" s="20" t="s">
         <v>37</v>
@@ -2011,7 +2032,7 @@
       <c r="A21" s="28"/>
       <c r="B21" s="28"/>
       <c r="C21" s="29" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D21" s="30" t="s">
         <v>28</v>
@@ -2020,25 +2041,25 @@
         <v>60</v>
       </c>
       <c r="F21" s="31" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G21" s="31" t="s">
         <v>31</v>
       </c>
       <c r="H21" s="32" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="I21" s="33" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="J21" s="34" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="K21" s="33" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="L21" s="35" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="M21" s="29" t="s">
         <v>37</v>
@@ -2065,13 +2086,13 @@
     </row>
     <row r="22">
       <c r="A22" s="37" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B22" s="40" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D22" s="21" t="s">
         <v>28</v>
@@ -2080,23 +2101,25 @@
         <v>60</v>
       </c>
       <c r="F22" s="22" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G22" s="22" t="s">
-        <v>128</v>
-      </c>
-      <c r="H22" s="23"/>
+        <v>129</v>
+      </c>
+      <c r="H22" s="32" t="s">
+        <v>130</v>
+      </c>
       <c r="I22" s="24" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="J22" s="25" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="K22" s="24" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="L22" s="26" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="M22" s="20" t="s">
         <v>37</v>
@@ -2125,7 +2148,7 @@
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
       <c r="C23" s="20" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D23" s="21" t="s">
         <v>28</v>
@@ -2134,23 +2157,25 @@
         <v>60</v>
       </c>
       <c r="F23" s="22" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="G23" s="22" t="s">
-        <v>128</v>
-      </c>
-      <c r="H23" s="23"/>
+        <v>137</v>
+      </c>
+      <c r="H23" s="32" t="s">
+        <v>130</v>
+      </c>
       <c r="I23" s="24" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="J23" s="25" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="K23" s="24" t="s">
         <v>35</v>
       </c>
       <c r="L23" s="26" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="M23" s="20" t="s">
         <v>37</v>
@@ -2179,7 +2204,7 @@
       <c r="A24" s="8"/>
       <c r="B24" s="8"/>
       <c r="C24" s="20" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D24" s="21" t="s">
         <v>28</v>
@@ -2188,23 +2213,25 @@
         <v>60</v>
       </c>
       <c r="F24" s="22" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="G24" s="22" t="s">
-        <v>128</v>
-      </c>
-      <c r="H24" s="23"/>
+        <v>143</v>
+      </c>
+      <c r="H24" s="32" t="s">
+        <v>130</v>
+      </c>
       <c r="I24" s="24" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="J24" s="25" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="K24" s="24" t="s">
         <v>35</v>
       </c>
       <c r="L24" s="26" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="M24" s="20" t="s">
         <v>37</v>
@@ -2233,7 +2260,7 @@
       <c r="A25" s="28"/>
       <c r="B25" s="28"/>
       <c r="C25" s="29" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="D25" s="30" t="s">
         <v>28</v>
@@ -2242,23 +2269,25 @@
         <v>60</v>
       </c>
       <c r="F25" s="31" t="s">
-        <v>139</v>
-      </c>
-      <c r="G25" s="31" t="s">
-        <v>128</v>
-      </c>
-      <c r="H25" s="32"/>
+        <v>142</v>
+      </c>
+      <c r="G25" s="22" t="s">
+        <v>148</v>
+      </c>
+      <c r="H25" s="32" t="s">
+        <v>130</v>
+      </c>
       <c r="I25" s="33" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="J25" s="34" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="K25" s="33" t="s">
         <v>35</v>
       </c>
       <c r="L25" s="35" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="M25" s="29" t="s">
         <v>37</v>

</xml_diff>